<commit_message>
Primera Version Estable de Presupuestos
</commit_message>
<xml_diff>
--- a/public/datos/partidas.xlsx
+++ b/public/datos/partidas.xlsx
@@ -15,15 +15,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
   <si>
-    <t>paredes</t>
+    <t>piso</t>
   </si>
   <si>
-    <t>2018-08-21 17:03:09</t>
+    <t>campo</t>
   </si>
   <si>
-    <t>2018-08-21 17:03:39</t>
+    <t>2018-08-27 22:11:40</t>
+  </si>
+  <si>
+    <t>2018-08-27 22:12:27</t>
   </si>
 </sst>
 </file>
@@ -362,7 +365,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -370,7 +373,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:16">
       <c r="A1">
         <v>1</v>
       </c>
@@ -384,13 +387,40 @@
         <v>1</v>
       </c>
       <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1">
         <v>0</v>
       </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1">
+        <v>0</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1">
+        <v>0</v>
+      </c>
+      <c r="L1">
+        <v>0</v>
+      </c>
+      <c r="M1">
+        <v>136</v>
+      </c>
+      <c r="N1">
+        <v>1</v>
+      </c>
+      <c r="O1" t="s">
         <v>2</v>
+      </c>
+      <c r="P1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios de exportacion e importacion
</commit_message>
<xml_diff>
--- a/public/datos/partidas.xlsx
+++ b/public/datos/partidas.xlsx
@@ -26,7 +26,7 @@
     <t>2018-08-27 22:11:40</t>
   </si>
   <si>
-    <t>2018-08-27 22:12:27</t>
+    <t>2018-09-03 22:04:13</t>
   </si>
 </sst>
 </file>
@@ -365,7 +365,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -373,7 +373,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:20">
       <c r="A1">
         <v>1</v>
       </c>
@@ -421,6 +421,18 @@
       </c>
       <c r="P1" t="s">
         <v>3</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1">
+        <v>0</v>
+      </c>
+      <c r="S1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios de Exportación y modificaciones de nombres de partidas
</commit_message>
<xml_diff>
--- a/public/datos/partidas.xlsx
+++ b/public/datos/partidas.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
   <si>
     <t>tomas 220v</t>
   </si>
@@ -26,27 +26,7 @@
     <t>2018-09-01 15:25:31</t>
   </si>
   <si>
-    <t>2018-09-10 21:14:05</t>
-  </si>
-  <si>
-    <t>&lt;h2 style="text-align: center;"&gt;T&amp;iacute;tulo&lt;/h2&gt;
-&lt;p&gt;P&amp;aacute;rrafos&lt;/p&gt;
-&lt;ul&gt;
-&lt;li&gt;Listas&lt;/li&gt;
-&lt;li&gt;Listas&lt;/li&gt;
-&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>#48abe6</t>
-  </si>
-  <si>
-    <t>Puertas</t>
-  </si>
-  <si>
-    <t>2018-09-10 21:14:20</t>
-  </si>
-  <si>
-    <t>2018-09-10 21:15:49</t>
+    <t>2018-09-11 18:52:04</t>
   </si>
   <si>
     <t>#ffffff</t>
@@ -388,7 +368,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,7 +414,7 @@
         <v>0</v>
       </c>
       <c r="M1">
-        <v>178.72</v>
+        <v>1307.236</v>
       </c>
       <c r="N1">
         <v>1</v>
@@ -445,76 +425,8 @@
       <c r="P1" t="s">
         <v>3</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>4</v>
-      </c>
-      <c r="V1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22">
-      <c r="A2">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>69.23</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2" t="s">
-        <v>7</v>
-      </c>
-      <c r="P2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>1</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2" t="s">
-        <v>1</v>
-      </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="V2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>